<commit_message>
Valida que a soma dos números de casos/mortes bate com os valores totais informados
</commit_message>
<xml_diff>
--- a/covid19/tests/data/sample-PR.xlsx
+++ b/covid19/tests/data/sample-PR.xlsx
@@ -67,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,7 +152,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -178,10 +179,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>